<commit_message>
make new imperial data
</commit_message>
<xml_diff>
--- a/R/data_refs/refbyhand_california-healthy-soils.xlsx
+++ b/R/data_refs/refbyhand_california-healthy-soils.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\alfalfa\R\data_refs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E840C3-9B6D-4BFF-97B1-D15171E7295A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26A4FB5-A504-431D-A01F-58AD65A06745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26B620E9-997F-4CCA-BF0B-BA9A66B0962F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="30">
   <si>
     <t>Manually creating a list of co2 impacts from CA Healthy Soils</t>
   </si>
@@ -84,6 +84,48 @@
   </si>
   <si>
     <t>no carbon credit</t>
+  </si>
+  <si>
+    <t>imperial</t>
+  </si>
+  <si>
+    <t>alameda</t>
+  </si>
+  <si>
+    <t>alpine</t>
+  </si>
+  <si>
+    <t>san bernardino</t>
+  </si>
+  <si>
+    <t>merced</t>
+  </si>
+  <si>
+    <t>inyo</t>
+  </si>
+  <si>
+    <t>riverside</t>
+  </si>
+  <si>
+    <t>san joaquin</t>
+  </si>
+  <si>
+    <t>fresno</t>
+  </si>
+  <si>
+    <t>shasta</t>
+  </si>
+  <si>
+    <t>lassen</t>
+  </si>
+  <si>
+    <t>kern</t>
+  </si>
+  <si>
+    <t>Residue and Tillage Management (CPS 329) - no-till</t>
+  </si>
+  <si>
+    <t>Residue and Tillage Management (CPS 345) - reduced till</t>
   </si>
 </sst>
 </file>
@@ -435,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{518DCD56-FF5D-4A7C-B0C4-70F0BCC09D49}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,24 +523,21 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
       <c r="D7">
-        <v>0.21</v>
+        <v>0.26</v>
       </c>
       <c r="E7">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -515,10 +554,10 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D9">
-        <v>0.26</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -529,13 +568,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D10">
-        <v>0.86</v>
+        <v>0.42</v>
       </c>
       <c r="E10">
-        <v>0.22</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -543,41 +582,41 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="D12">
-        <v>0.26</v>
+        <v>0.21</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="D13">
-        <v>0.86</v>
+        <v>1.21</v>
       </c>
       <c r="E13">
-        <v>0.22</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -585,13 +624,13 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D14">
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -599,13 +638,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D15">
-        <v>1.21</v>
+        <v>0.15</v>
       </c>
       <c r="E15">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -613,12 +652,645 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E16">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>0.26</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>0.7</v>
+      </c>
+      <c r="E18">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <v>0.23</v>
+      </c>
+      <c r="E20">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21">
+        <v>0.1</v>
+      </c>
+      <c r="E21">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22">
+        <v>0.26</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>1.26</v>
+      </c>
+      <c r="E23">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25">
+        <v>0.21</v>
+      </c>
+      <c r="E25">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>0.78</v>
+      </c>
+      <c r="E26">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28">
+        <v>0.26</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>0.78</v>
+      </c>
+      <c r="E29">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31">
+        <v>0.26</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32">
+        <v>0.86</v>
+      </c>
+      <c r="E32">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34">
+        <v>0.26</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35">
+        <v>0.78</v>
+      </c>
+      <c r="E35">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37">
+        <v>0.26</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38">
+        <v>0.7</v>
+      </c>
+      <c r="E38">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40">
+        <v>0.26</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41">
+        <v>0.86</v>
+      </c>
+      <c r="E41">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43">
+        <v>0.26</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44">
+        <v>0.86</v>
+      </c>
+      <c r="E44">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46">
+        <v>0.21</v>
+      </c>
+      <c r="E46">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47">
+        <v>1.19</v>
+      </c>
+      <c r="E47">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49">
+        <v>0.26</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50">
+        <v>1.19</v>
+      </c>
+      <c r="E50">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52">
+        <v>0.26</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53">
+        <v>0.86</v>
+      </c>
+      <c r="E53">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" t="s">
+        <v>28</v>
+      </c>
+      <c r="D55">
+        <v>0.42</v>
+      </c>
+      <c r="E55">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56">
+        <v>0.21</v>
+      </c>
+      <c r="E56">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57">
+        <v>0.86</v>
+      </c>
+      <c r="E57">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59">
+        <v>0.26</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60">
+        <v>0.86</v>
+      </c>
+      <c r="E60">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
         <v>0</v>
       </c>
     </row>

</xml_diff>